<commit_message>
SPT 3.5 template update
</commit_message>
<xml_diff>
--- a/Projects/RINIELSENUS/Data/Template_2018_SPT.xlsx
+++ b/Projects/RINIELSENUS/Data/Template_2018_SPT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatieSchrage\Documents\Mars SPT_Year End 2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59261978-E8CB-41C6-8EBC-D3DBB82BFEE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83760FB-6336-4AAA-B206-476592E8D394}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="894" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,6 +37,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hierarchy!$A$1:$K$68</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">NBIL!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">sales!$A$1:$I$13</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="8">NBIL!$A$1:$G$1</definedName>
     <definedName name="_FilterDatabase_0_0" localSheetId="8">NBIL!$A$1:$G$1</definedName>
     <definedName name="count">#REF!</definedName>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4390" uniqueCount="749">
   <si>
     <t>Set name</t>
   </si>
@@ -2301,6 +2302,9 @@
   </si>
   <si>
     <t>DENTASTIX FRESH BISCUITS,DENTASTIX FRESH BITES,DENTASTIX PUPPY</t>
+  </si>
+  <si>
+    <t>Updated SOA in sales sheet</t>
   </si>
 </sst>
 </file>
@@ -2504,7 +2508,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2650,6 +2654,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53" customBuiltin="1"/>
@@ -3073,7 +3079,7 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3378,6 +3384,17 @@
       </c>
       <c r="L8" s="30">
         <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="67">
+        <v>43389</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>748</v>
+      </c>
+      <c r="D9" t="s">
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -8414,8 +8431,8 @@
     <col min="6" max="6" width="15.5703125"/>
     <col min="7" max="7" width="12.140625"/>
     <col min="8" max="8" width="35.140625"/>
-    <col min="9" max="9" width="7.5703125"/>
-    <col min="10" max="1025" width="8.5703125"/>
+    <col min="9" max="9" width="8.5703125" style="20"/>
+    <col min="10" max="1024" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -8443,7 +8460,7 @@
       <c r="H1" t="s">
         <v>131</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="20" t="s">
         <v>132</v>
       </c>
     </row>
@@ -8473,7 +8490,7 @@
         <v>139</v>
       </c>
       <c r="I2" s="20">
-        <v>8.6737796582475806</v>
+        <v>1.5903014132858266E-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8499,7 +8516,7 @@
         <v>140</v>
       </c>
       <c r="I3" s="20">
-        <v>9.8200403982364506</v>
+        <v>8.3109300950776834</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -8528,7 +8545,7 @@
         <v>139</v>
       </c>
       <c r="I4" s="20">
-        <v>20.432023824358101</v>
+        <v>14.880668134877203</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8554,7 +8571,7 @@
         <v>140</v>
       </c>
       <c r="I5" s="20">
-        <v>19.133694047768198</v>
+        <v>18.591870167348944</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8583,7 +8600,7 @@
         <v>143</v>
       </c>
       <c r="I6" s="20">
-        <v>25.96987416724</v>
+        <v>19.135424973090711</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -8609,7 +8626,7 @@
         <v>144</v>
       </c>
       <c r="I7" s="20">
-        <v>5.1243043431852797</v>
+        <v>5.0835164946496638</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -8638,7 +8655,7 @@
         <v>143</v>
       </c>
       <c r="I8" s="20">
-        <v>32.470822099608903</v>
+        <v>28.598878735426158</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8664,7 +8681,7 @@
         <v>144</v>
       </c>
       <c r="I9" s="20">
-        <v>12.513043525293901</v>
+        <v>12.599931807229373</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -8684,7 +8701,7 @@
         <v>136</v>
       </c>
       <c r="I10" s="20">
-        <v>21.0672412618006</v>
+        <v>20.065653054711159</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -8704,7 +8721,7 @@
         <v>136</v>
       </c>
       <c r="I11" s="20">
-        <v>24.421974816201399</v>
+        <v>25.969597205754312</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -8724,7 +8741,7 @@
         <v>136</v>
       </c>
       <c r="I12" s="20">
-        <v>52.596491548543902</v>
+        <v>51.589719027449142</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -8744,10 +8761,11 @@
         <v>136</v>
       </c>
       <c r="I13" s="20">
-        <v>61.126383122607002</v>
+        <v>60.991102411080547</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I13" xr:uid="{2817B11E-52EF-467C-B96E-E84BBD14A674}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>